<commit_message>
playing with heat map
</commit_message>
<xml_diff>
--- a/data/xlsx/03022019.xlsx
+++ b/data/xlsx/03022019.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachelli/Desktop/SUSA/[s19] web dev/susa-data-viz/data/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachelli/Desktop/SUSA/susa-data-viz/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F85B9D-2D1A-4A4F-8420-22E63C9B77D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D21A1C-F443-E440-9BBC-C693346D7A52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="440" windowWidth="14860" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -261,7 +261,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -314,7 +314,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -918,8 +918,12 @@
       <c r="E10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10">
+        <v>37.869249000000003</v>
+      </c>
+      <c r="G10">
+        <v>-122.25967</v>
+      </c>
       <c r="H10" s="3" t="s">
         <v>77</v>
       </c>

</xml_diff>